<commit_message>
added data provided by Tej, Combined Crime Analysis with Zip Code and removed Creime Analysis, removed count_to_bar
</commit_message>
<xml_diff>
--- a/ZipCodeLocator/CountOfCrimes.xlsx
+++ b/ZipCodeLocator/CountOfCrimes.xlsx
@@ -14,12 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
-  <si>
-    <t>Zipcode</t>
-  </si>
-  <si>
-    <t>Primary Type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="31">
+  <si>
+    <t>GEOID10</t>
+  </si>
+  <si>
+    <t>Primary_Ty</t>
+  </si>
+  <si>
+    <t>CRIMINAL TRESPASS</t>
+  </si>
+  <si>
+    <t>DECEPTIVE PRACTICE</t>
+  </si>
+  <si>
+    <t>THEFT</t>
+  </si>
+  <si>
+    <t>ARSON</t>
   </si>
   <si>
     <t>ASSAULT</t>
@@ -34,43 +46,67 @@
     <t>CRIMINAL DAMAGE</t>
   </si>
   <si>
-    <t>DECEPTIVE PRACTICE</t>
+    <t>CRIMINAL SEXUAL ASSAULT</t>
   </si>
   <si>
     <t>HOMICIDE</t>
   </si>
   <si>
+    <t>INTERFERENCE WITH PUBLIC OFFICER</t>
+  </si>
+  <si>
+    <t>INTIMIDATION</t>
+  </si>
+  <si>
+    <t>KIDNAPPING</t>
+  </si>
+  <si>
+    <t>LIQUOR LAW VIOLATION</t>
+  </si>
+  <si>
     <t>MOTOR VEHICLE THEFT</t>
   </si>
   <si>
+    <t>NARCOTICS</t>
+  </si>
+  <si>
     <t>OFFENSE INVOLVING CHILDREN</t>
   </si>
   <si>
     <t>OTHER OFFENSE</t>
   </si>
   <si>
+    <t>PUBLIC INDECENCY</t>
+  </si>
+  <si>
     <t>ROBBERY</t>
   </si>
   <si>
-    <t>THEFT</t>
+    <t>SEX OFFENSE</t>
+  </si>
+  <si>
+    <t>STALKING</t>
   </si>
   <si>
     <t>WEAPONS VIOLATION</t>
   </si>
   <si>
-    <t>CRIMINAL SEXUAL ASSAULT</t>
-  </si>
-  <si>
-    <t>CRIMINAL TRESPASS</t>
-  </si>
-  <si>
-    <t>NARCOTICS</t>
-  </si>
-  <si>
-    <t>SEX OFFENSE</t>
-  </si>
-  <si>
-    <t>KIDNAPPING</t>
+    <t>CONCEALED CARRY LICENSE VIOLATION</t>
+  </si>
+  <si>
+    <t>GAMBLING</t>
+  </si>
+  <si>
+    <t>NON-CRIMINAL</t>
+  </si>
+  <si>
+    <t>OBSCENITY</t>
+  </si>
+  <si>
+    <t>PUBLIC PEACE VIOLATION</t>
+  </si>
+  <si>
+    <t>HUMAN TRAFFICKING</t>
   </si>
 </sst>
 </file>
@@ -428,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,13 +483,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>46394</v>
+        <v>60611</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -462,7 +498,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -471,16 +507,18 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>60615</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -489,7 +527,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -498,7 +536,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -507,7 +545,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -516,7 +554,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -525,251 +563,249 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>60617</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
         <v>2</v>
-      </c>
-      <c r="C14">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C17">
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
         <v>6</v>
-      </c>
-      <c r="C20">
-        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C22">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C25">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>11</v>
+        <v>766</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1">
+        <v>60617</v>
+      </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C28">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1">
-        <v>60633</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C30">
-        <v>15</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C31">
-        <v>26</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32">
         <v>4</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C33">
-        <v>14</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>7</v>
+        <v>371</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -778,62 +814,1595 @@
     <row r="38" spans="1:3">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C38">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C40">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C42">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52">
         <v>13</v>
       </c>
-      <c r="C43">
-        <v>1</v>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1">
+        <v>60619</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C75">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1">
+        <v>60628</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C85">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C98">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1">
+        <v>60633</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C106">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C111">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C114">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C117">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C121">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="1">
+        <v>60637</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C125">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C129">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C130">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C131">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C135">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C136">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C137">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C138">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C139">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C140">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C141">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C142">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C143">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C144">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="1">
+        <v>60649</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C146">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C148">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C150">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C151">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="1"/>
+      <c r="B153" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="1"/>
+      <c r="B154" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="1"/>
+      <c r="B155" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C159">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="1"/>
+      <c r="B160" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C160">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C162">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C163">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C164">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="1"/>
+      <c r="B165" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C165">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C166">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C167">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C168">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C169">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="1">
+        <v>60653</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C172">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C173">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C174">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C175">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C176">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C177">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C178">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C181">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C182">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="1"/>
+      <c r="B183" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C184">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="1"/>
+      <c r="B185" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C185">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="1"/>
+      <c r="B186" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="1"/>
+      <c r="B187" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C187">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="1"/>
+      <c r="B188" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C188">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="1"/>
+      <c r="B189" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C189">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="1"/>
+      <c r="B190" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C190">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="1"/>
+      <c r="B191" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C191">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="1">
+        <v>60827</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="1"/>
+      <c r="B193" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C193">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" s="1"/>
+      <c r="B194" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C194">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" s="1"/>
+      <c r="B195" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C195">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="1"/>
+      <c r="B196" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C196">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="1"/>
+      <c r="B197" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C197">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="1"/>
+      <c r="B198" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C198">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="1"/>
+      <c r="B199" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="1"/>
+      <c r="B200" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="1"/>
+      <c r="B201" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="1"/>
+      <c r="B202" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C202">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="1"/>
+      <c r="B203" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="1"/>
+      <c r="B204" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C204">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="1"/>
+      <c r="B205" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C205">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="1"/>
+      <c r="B206" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="1"/>
+      <c r="B207" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C207">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="1"/>
+      <c r="B208" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C208">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="1"/>
+      <c r="B209" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="1"/>
+      <c r="B210" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C210">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="1"/>
+      <c r="B211" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C211">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A29"/>
-    <mergeCell ref="A30:A43"/>
+  <mergeCells count="10">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A27"/>
+    <mergeCell ref="A28:A54"/>
+    <mergeCell ref="A55:A78"/>
+    <mergeCell ref="A79:A98"/>
+    <mergeCell ref="A99:A121"/>
+    <mergeCell ref="A122:A144"/>
+    <mergeCell ref="A145:A169"/>
+    <mergeCell ref="A170:A191"/>
+    <mergeCell ref="A192:A211"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>